<commit_message>
User Story 08 - Birth Before Marriage
</commit_message>
<xml_diff>
--- a/TeamArunChristianJeffreyLeenaReport.xlsx
+++ b/TeamArunChristianJeffreyLeenaReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenadomadia/Documents/repos/GEDCOM-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\SSW 555\GEDCOM-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DF5B0B-1211-3347-91A5-23E4853424F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75017D20-53E7-4D3C-B044-65E60715FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="920" windowWidth="27720" windowHeight="15460" activeTab="7" xr2:uid="{F28C54A4-57B8-3C4B-A7BE-8D82FD74D0C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{F28C54A4-57B8-3C4B-A7BE-8D82FD74D0C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="146">
   <si>
     <t>Initials</t>
   </si>
@@ -906,13 +904,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -929,7 +927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -946,7 +944,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -963,7 +961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -980,7 +978,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -997,7 +995,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1024,13 +1022,13 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="28.375" customWidth="1"/>
+    <col min="4" max="4" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1047,7 +1045,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1064,7 +1062,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1081,7 +1079,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1095,7 +1093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1109,7 +1107,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>44</v>
       </c>
@@ -1131,7 +1129,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>47</v>
       </c>
@@ -1139,7 +1137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1153,7 +1151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>53</v>
       </c>
@@ -1161,7 +1159,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1169,7 +1167,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>59</v>
       </c>
@@ -1177,7 +1175,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>62</v>
       </c>
@@ -1185,7 +1183,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>65</v>
       </c>
@@ -1193,7 +1191,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>68</v>
       </c>
@@ -1201,7 +1199,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>71</v>
       </c>
@@ -1209,7 +1207,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1226,7 +1224,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>77</v>
       </c>
@@ -1234,7 +1232,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>80</v>
       </c>
@@ -1242,7 +1240,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>83</v>
       </c>
@@ -1250,7 +1248,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>86</v>
       </c>
@@ -1258,7 +1256,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>89</v>
       </c>
@@ -1266,7 +1264,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1283,7 +1281,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>95</v>
       </c>
@@ -1291,7 +1289,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>98</v>
       </c>
@@ -1299,7 +1297,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>101</v>
       </c>
@@ -1307,7 +1305,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>104</v>
       </c>
@@ -1315,7 +1313,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>107</v>
       </c>
@@ -1323,7 +1321,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>110</v>
       </c>
@@ -1331,7 +1329,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>113</v>
       </c>
@@ -1339,7 +1337,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>116</v>
       </c>
@@ -1347,7 +1345,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>119</v>
       </c>
@@ -1355,7 +1353,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>122</v>
       </c>
@@ -1376,13 +1374,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1405,7 +1403,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -1419,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -1427,7 +1425,7 @@
         <v>44480</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -1435,7 +1433,7 @@
         <v>44494</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -1443,7 +1441,7 @@
         <v>44508</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -1460,16 +1458,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BC7DFE-C60F-9C48-B5C3-3956B3F33744}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1498,7 +1496,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -1527,7 +1525,7 @@
         <v>44466</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1556,7 +1554,7 @@
         <v>44472</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -1573,7 +1571,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1583,14 +1581,26 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
       <c r="E5">
         <v>30</v>
       </c>
       <c r="F5">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+      <c r="I5" s="11">
+        <v>44472</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -1607,7 +1617,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1617,14 +1627,26 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
+      <c r="D7" t="s">
+        <v>125</v>
+      </c>
       <c r="E7">
         <v>40</v>
       </c>
       <c r="F7">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>25</v>
+      </c>
+      <c r="I7" s="11">
+        <v>44473</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>74</v>
       </c>
@@ -1653,7 +1675,7 @@
         <v>44466</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>92</v>
       </c>
@@ -1682,11 +1704,11 @@
         <v>44466</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>
@@ -1703,12 +1725,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1750,12 +1772,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1797,12 +1819,12 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1840,17 +1862,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7771E13B-00CA-A14A-9142-77D98EE1784C}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="69.33203125" customWidth="1"/>
+    <col min="3" max="3" width="69.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1861,7 +1883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>29</v>
       </c>
@@ -1872,7 +1894,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
@@ -1883,7 +1905,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1894,7 +1916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>38</v>
       </c>
@@ -1905,7 +1927,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>41</v>
       </c>
@@ -1916,7 +1938,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
@@ -1927,7 +1949,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>47</v>
       </c>
@@ -1938,7 +1960,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>50</v>
       </c>
@@ -1949,7 +1971,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>53</v>
       </c>
@@ -1960,7 +1982,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1971,7 +1993,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -1982,7 +2004,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
@@ -1993,7 +2015,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>65</v>
       </c>
@@ -2004,7 +2026,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>68</v>
       </c>
@@ -2015,7 +2037,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>71</v>
       </c>
@@ -2026,7 +2048,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>74</v>
       </c>
@@ -2037,7 +2059,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>77</v>
       </c>
@@ -2048,7 +2070,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>80</v>
       </c>
@@ -2059,7 +2081,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>83</v>
       </c>
@@ -2070,7 +2092,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>86</v>
       </c>
@@ -2081,7 +2103,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>89</v>
       </c>
@@ -2092,7 +2114,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>92</v>
       </c>
@@ -2103,7 +2125,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
@@ -2114,7 +2136,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>98</v>
       </c>
@@ -2125,7 +2147,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>101</v>
       </c>
@@ -2136,7 +2158,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>104</v>
       </c>
@@ -2147,7 +2169,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>107</v>
       </c>
@@ -2158,7 +2180,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>110</v>
       </c>
@@ -2169,7 +2191,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>113</v>
       </c>
@@ -2180,7 +2202,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>116</v>
       </c>
@@ -2191,7 +2213,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>119</v>
       </c>
@@ -2202,7 +2224,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>122</v>
       </c>
@@ -2213,52 +2235,52 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>

</xml_diff>

<commit_message>
Changes needed for US08 and test cases added
</commit_message>
<xml_diff>
--- a/TeamArunChristianJeffreyLeenaReport.xlsx
+++ b/TeamArunChristianJeffreyLeenaReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\SSW 555\GEDCOM-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75017D20-53E7-4D3C-B044-65E60715FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D9061C-2A34-4D7B-95FF-7780096C15F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{F28C54A4-57B8-3C4B-A7BE-8D82FD74D0C2}"/>
   </bookViews>
@@ -1459,7 +1459,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1640,7 +1640,7 @@
         <v>35</v>
       </c>
       <c r="H7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I7" s="11">
         <v>44473</v>

</xml_diff>

<commit_message>
Removing changes to Excel
</commit_message>
<xml_diff>
--- a/TeamArunChristianJeffreyLeenaReport.xlsx
+++ b/TeamArunChristianJeffreyLeenaReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\SSW 555\GEDCOM-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leenadomadia/Documents/repos/GEDCOM-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D9061C-2A34-4D7B-95FF-7780096C15F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2903B69C-1FDC-CB41-82AF-59531A0E8376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{F28C54A4-57B8-3C4B-A7BE-8D82FD74D0C2}"/>
+    <workbookView xWindow="720" yWindow="920" windowWidth="27720" windowHeight="15460" activeTab="3" xr2:uid="{F28C54A4-57B8-3C4B-A7BE-8D82FD74D0C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="146">
   <si>
     <t>Initials</t>
   </si>
@@ -904,13 +906,13 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -927,7 +929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -944,7 +946,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -961,7 +963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -978,7 +980,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -995,7 +997,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1022,13 +1024,13 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="28.375" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1045,7 +1047,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1062,7 +1064,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1079,7 +1081,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1093,7 +1095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1107,7 +1109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1121,7 +1123,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>44</v>
       </c>
@@ -1129,7 +1131,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>47</v>
       </c>
@@ -1137,7 +1139,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>53</v>
       </c>
@@ -1159,7 +1161,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1167,7 +1169,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>59</v>
       </c>
@@ -1175,7 +1177,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>62</v>
       </c>
@@ -1183,7 +1185,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>65</v>
       </c>
@@ -1191,7 +1193,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>68</v>
       </c>
@@ -1199,7 +1201,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>71</v>
       </c>
@@ -1207,7 +1209,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1224,7 +1226,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>77</v>
       </c>
@@ -1232,7 +1234,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>80</v>
       </c>
@@ -1240,7 +1242,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>83</v>
       </c>
@@ -1248,7 +1250,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>86</v>
       </c>
@@ -1256,7 +1258,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>89</v>
       </c>
@@ -1264,7 +1266,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1281,7 +1283,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>95</v>
       </c>
@@ -1289,7 +1291,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>98</v>
       </c>
@@ -1297,7 +1299,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>101</v>
       </c>
@@ -1305,7 +1307,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>104</v>
       </c>
@@ -1313,7 +1315,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>107</v>
       </c>
@@ -1321,7 +1323,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>110</v>
       </c>
@@ -1329,7 +1331,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>113</v>
       </c>
@@ -1337,7 +1339,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>116</v>
       </c>
@@ -1345,7 +1347,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>119</v>
       </c>
@@ -1353,7 +1355,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>122</v>
       </c>
@@ -1374,13 +1376,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="4" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1403,7 +1405,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -1417,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -1425,7 +1427,7 @@
         <v>44480</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -1433,7 +1435,7 @@
         <v>44494</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -1441,7 +1443,7 @@
         <v>44508</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -1459,15 +1461,15 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.875" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1496,7 +1498,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -1516,16 +1518,16 @@
         <v>30</v>
       </c>
       <c r="G2">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H2">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I2" s="11">
-        <v>44466</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44473</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1554,7 +1556,7 @@
         <v>44472</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>35</v>
       </c>
@@ -1564,14 +1566,26 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
       <c r="E4">
         <v>30</v>
       </c>
       <c r="F4">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" s="11">
+        <v>44472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1581,26 +1595,14 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>125</v>
-      </c>
       <c r="E5">
         <v>30</v>
       </c>
       <c r="F5">
         <v>45</v>
       </c>
-      <c r="G5">
-        <v>25</v>
-      </c>
-      <c r="H5">
-        <v>40</v>
-      </c>
-      <c r="I5" s="11">
-        <v>44472</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -1617,7 +1619,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1627,26 +1629,14 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>125</v>
-      </c>
       <c r="E7">
         <v>40</v>
       </c>
       <c r="F7">
         <v>60</v>
       </c>
-      <c r="G7">
-        <v>35</v>
-      </c>
-      <c r="H7">
-        <v>50</v>
-      </c>
-      <c r="I7" s="11">
-        <v>44473</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>74</v>
       </c>
@@ -1675,7 +1665,7 @@
         <v>44466</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>92</v>
       </c>
@@ -1704,11 +1694,11 @@
         <v>44466</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
     </row>
@@ -1725,12 +1715,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.875" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1772,12 +1762,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.875" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1819,12 +1809,12 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.875" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1862,17 +1852,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7771E13B-00CA-A14A-9142-77D98EE1784C}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="69.375" customWidth="1"/>
+    <col min="3" max="3" width="69.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -1883,7 +1873,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>29</v>
       </c>
@@ -1894,7 +1884,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
@@ -1905,7 +1895,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -1916,7 +1906,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>38</v>
       </c>
@@ -1927,7 +1917,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>41</v>
       </c>
@@ -1938,7 +1928,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
@@ -1949,7 +1939,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>47</v>
       </c>
@@ -1960,7 +1950,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>50</v>
       </c>
@@ -1971,7 +1961,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>53</v>
       </c>
@@ -1982,7 +1972,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1993,7 +1983,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -2004,7 +1994,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
@@ -2015,7 +2005,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>65</v>
       </c>
@@ -2026,7 +2016,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>68</v>
       </c>
@@ -2037,7 +2027,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>71</v>
       </c>
@@ -2048,7 +2038,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>74</v>
       </c>
@@ -2059,7 +2049,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>77</v>
       </c>
@@ -2070,7 +2060,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>80</v>
       </c>
@@ -2081,7 +2071,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>83</v>
       </c>
@@ -2092,7 +2082,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>86</v>
       </c>
@@ -2103,7 +2093,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>89</v>
       </c>
@@ -2114,7 +2104,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>92</v>
       </c>
@@ -2125,7 +2115,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>95</v>
       </c>
@@ -2136,7 +2126,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>98</v>
       </c>
@@ -2147,7 +2137,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>101</v>
       </c>
@@ -2158,7 +2148,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>104</v>
       </c>
@@ -2169,7 +2159,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>107</v>
       </c>
@@ -2180,7 +2170,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>110</v>
       </c>
@@ -2191,7 +2181,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>113</v>
       </c>
@@ -2202,7 +2192,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>116</v>
       </c>
@@ -2213,7 +2203,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>119</v>
       </c>
@@ -2224,7 +2214,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>122</v>
       </c>
@@ -2235,52 +2225,52 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="4"/>

</xml_diff>